<commit_message>
updated READMEs of ios & nodejs
</commit_message>
<xml_diff>
--- a/nodejs/docimg/flow.xlsx
+++ b/nodejs/docimg/flow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/utetsuo/workplace/amazonpay-sample-app-v2/nodejs/docimg/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/utetsuo/workspace/dev/maxopus/amazonpaycpsp-gmosampleapp-2step/nodejs/docimg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B137C728-A906-7F46-A515-FC26D37B4695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB09D28-D223-5941-B1A3-B083FD0CB903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11620" yWindow="-22540" windowWidth="30140" windowHeight="21120" xr2:uid="{768BDD66-EE21-F447-8F0F-031CD939AA71}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" xr2:uid="{768BDD66-EE21-F447-8F0F-031CD939AA71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,23 +80,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rectangle 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20D29F9D-8BC3-5044-8D2E-73B19F00CF3C}"/>
+        <xdr:cNvPr id="24" name="Rounded Rectangle 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15B570EA-CC3F-7043-8165-1E5D7ED7BB9C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -104,150 +104,256 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3784600" y="215900"/>
-          <a:ext cx="4902200" cy="4203700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent4">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent4"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent4"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
+          <a:off x="13373100" y="11328400"/>
+          <a:ext cx="2832100" cy="4622800"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 4327"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="accent2"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="b"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Amazon側の画面</a:t>
-          </a:r>
+            <a:t>Secure</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>WebView</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Rounded Rectangle 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EF6C2F6-5B2D-3345-B8DA-15FB66ED2B59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3606800" y="11315700"/>
+          <a:ext cx="7493000" cy="4635500"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 4327"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="accent2"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Secure</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>WebView</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="86" name="Group 85">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A269E975-CDED-CE2D-0AEB-27F26B01C2C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="11252200" y="11709400"/>
+          <a:ext cx="2120900" cy="3632200"/>
+          <a:chOff x="9906000" y="16459200"/>
+          <a:chExt cx="5655022" cy="10058400"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="82" name="Picture 81">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{018B5D5E-66A0-B633-D702-589345742CAA}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9906000" y="16459200"/>
+            <a:ext cx="5655022" cy="10058400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="85" name="Picture 84">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95B676A7-5570-5C08-F6CA-DBF4AFC60B43}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10223500" y="23050500"/>
+            <a:ext cx="5003800" cy="3429000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>723899</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>203808</xdr:colOff>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{090609E8-FD75-1249-9E0D-874E1A8BFAB6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1663700" y="622300"/>
-          <a:ext cx="1536700" cy="3454400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CA3B84C-35AC-9E4A-9ABE-BCA40CE8AA32}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4140200" y="622300"/>
-          <a:ext cx="1587500" cy="3467100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19F69E96-CE27-C644-9166-8A3AC1D011E9}"/>
+        <xdr:cNvPr id="74" name="Picture 73">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D6B898B-B599-0801-10EE-B92B76F0EDE5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -257,6 +363,201 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1549399" y="11772900"/>
+          <a:ext cx="1956409" cy="3479800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20D29F9D-8BC3-5044-8D2E-73B19F00CF3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3784600" y="215900"/>
+          <a:ext cx="4902200" cy="4203700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Amazon側の画面</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{090609E8-FD75-1249-9E0D-874E1A8BFAB6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1663700" y="622300"/>
+          <a:ext cx="1536700" cy="3454400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CA3B84C-35AC-9E4A-9ABE-BCA40CE8AA32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4140200" y="622300"/>
+          <a:ext cx="1587500" cy="3467100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19F69E96-CE27-C644-9166-8A3AC1D011E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -319,7 +620,7 @@
           </xdr:cNvPicPr>
         </xdr:nvPicPr>
         <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
           <a:stretch>
             <a:fillRect/>
           </a:stretch>
@@ -348,7 +649,7 @@
           </xdr:cNvPicPr>
         </xdr:nvPicPr>
         <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
           <a:stretch>
             <a:fillRect/>
           </a:stretch>
@@ -456,7 +757,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -500,7 +801,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1136,7 +1437,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1243,7 +1544,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1287,7 +1588,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1413,7 +1714,7 @@
           </xdr:cNvPicPr>
         </xdr:nvPicPr>
         <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
           <a:stretch>
             <a:fillRect/>
           </a:stretch>
@@ -1442,7 +1743,7 @@
           </xdr:cNvPicPr>
         </xdr:nvPicPr>
         <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
           <a:stretch>
             <a:fillRect/>
           </a:stretch>
@@ -1487,7 +1788,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1531,7 +1832,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2563,13 +2864,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>137</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>520701</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>145</xdr:row>
       <xdr:rowOff>65079</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -2585,7 +2886,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2133600" y="11353800"/>
+          <a:off x="2133600" y="28028900"/>
           <a:ext cx="863601" cy="1512879"/>
           <a:chOff x="3302000" y="11582400"/>
           <a:chExt cx="863601" cy="1512879"/>
@@ -2605,7 +2906,7 @@
           </xdr:cNvPicPr>
         </xdr:nvPicPr>
         <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
           <a:stretch>
             <a:fillRect/>
           </a:stretch>
@@ -2634,7 +2935,7 @@
           </xdr:cNvPicPr>
         </xdr:nvPicPr>
         <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
           <a:stretch>
             <a:fillRect/>
           </a:stretch>
@@ -2656,13 +2957,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>135</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>152</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2679,7 +2980,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2694,6 +2995,2563 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A7A56EB-BFEF-0B45-9130-65AD232A7D73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2933700" y="7823200"/>
+          <a:ext cx="1193800" cy="82550"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="Rectangle 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2AACA59-CB71-CE49-8D0C-3195B9E3F302}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3784600" y="11379200"/>
+          <a:ext cx="4902200" cy="4203700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Amazon側の画面</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="Rectangle 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99FD6C89-2968-A04C-80F8-83F1E56712E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13462000" y="11379200"/>
+          <a:ext cx="2603500" cy="4203700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Amazon側の画面</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="Rectangle 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C8635E4-126A-1747-865B-D2AE1D842886}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3213100" y="13030200"/>
+          <a:ext cx="673100" cy="596900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>①</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="Rectangle 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{685749D9-BC13-5145-BB32-874DBDAB3430}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8267700" y="12954000"/>
+          <a:ext cx="863600" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>②-1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="61" name="Straight Arrow Connector 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D5B64B3-16F1-5A4C-B504-29EFCCB876BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:endCxn id="95" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12903200" y="13481050"/>
+          <a:ext cx="914400" cy="1631950"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="62" name="Rectangle 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E3AC968-5A73-4646-B995-913C0E5B5899}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12954000" y="13703300"/>
+          <a:ext cx="673100" cy="596900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>③</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="67" name="Rectangle 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E65C2049-6E64-E44D-9585-45D404F52B94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15760700" y="13004800"/>
+          <a:ext cx="673100" cy="596900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>④</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="68" name="Rectangle 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90513299-9410-B84F-801C-450FC9C66D66}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="11404600"/>
+          <a:ext cx="1663700" cy="596900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>カートページ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="69" name="Rectangle 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3F01EC5-2E61-7148-881B-20A2860DAA1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11658600" y="11341100"/>
+          <a:ext cx="1358900" cy="596900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>購入ページ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="70" name="Rectangle 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{769A9CB0-C45F-C24A-B356-DBE540515FCA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16598900" y="11391900"/>
+          <a:ext cx="1587500" cy="596900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>Thanksページ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>711199</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="71" name="Straight Arrow Connector 70">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBF9EDCE-7DDB-0A41-AAA5-EEDA19D35DB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="76" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2971800" y="13474700"/>
+          <a:ext cx="1041399" cy="165100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>711199</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>205388</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="76" name="Picture 75">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E47A485-CAE4-2019-34EE-6281C85FE8CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4013199" y="11722100"/>
+          <a:ext cx="1970689" cy="3505200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>103789</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="79" name="Picture 78">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E6DF639-CE5C-F082-16CF-F1F836982BB0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6388100" y="11722100"/>
+          <a:ext cx="1970689" cy="3505200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="Straight Arrow Connector 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6594A7AE-06B5-6A4B-B4D6-5810C8713492}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:endCxn id="79" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5613400" y="13474700"/>
+          <a:ext cx="774700" cy="812800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>182338</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="81" name="Picture 80">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00DD3808-3ACA-C838-81D6-669969AB3D7C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9080500" y="11785600"/>
+          <a:ext cx="1930400" cy="3433538"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="Straight Arrow Connector 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{877C8C68-B9F0-6B41-A039-621D8F7D7B90}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="82" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10541000" y="13182600"/>
+          <a:ext cx="711200" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>91169</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="90" name="Straight Arrow Connector 89">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE2A6CD4-D5A4-BD4E-AC83-BC482EE2B682}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="81" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7975600" y="13502369"/>
+          <a:ext cx="1104900" cy="73931"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="93" name="Rectangle 92">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CABA52A4-73BA-F043-AFF7-ACFB73275039}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10287000" y="13322300"/>
+          <a:ext cx="863600" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>②-2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>125210</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="95" name="Picture 94">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F0263CA-3B0E-2D98-CA25-5C4535F635EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13817600" y="11709400"/>
+          <a:ext cx="1992110" cy="3543300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="63" name="Straight Arrow Connector 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2F9277F-8E9D-5A49-B993-671D2DD73356}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15633700" y="13506450"/>
+          <a:ext cx="838200" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>8805</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="97" name="Picture 96">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DD175F7-3367-D175-BC9A-FD57C6E19B83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16459200" y="11747500"/>
+          <a:ext cx="1968500" cy="3501305"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>154331</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E83A640-345C-B340-A883-C96427C88987}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1651000" y="17424400"/>
+          <a:ext cx="2171700" cy="3862731"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="Rectangle 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCC71479-C289-D042-B8FE-653A6E991D8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2133600" y="17018000"/>
+          <a:ext cx="1358900" cy="596900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>購入ページ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="Rounded Rectangle 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C34CB6A-B9E1-0E40-8509-0663CF135DF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4076700" y="16878300"/>
+          <a:ext cx="5232400" cy="4635500"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 4327"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="accent2"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Secure</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>WebView</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="72" name="Rectangle 71">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C6DC84C-B532-324B-BDEE-C72D6D455FB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4305300" y="16941800"/>
+          <a:ext cx="2590800" cy="4203700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Amazon側の画面</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="73" name="Rectangle 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15F533CF-E8C0-7A48-81B8-362F2A8B05AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6477000" y="18516600"/>
+          <a:ext cx="863600" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>②-1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>789589</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="75" name="Picture 74">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29337C1A-4C39-2D4B-8CAC-40581D911D8B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4597400" y="17284700"/>
+          <a:ext cx="1970689" cy="3505200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>55338</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="77" name="Picture 76">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45FDB9AA-0CEF-0048-842C-DBCCF5EB4FB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7289800" y="17348200"/>
+          <a:ext cx="1930400" cy="3433538"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="78" name="Straight Arrow Connector 77">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{460EDAFF-7668-BB41-B00D-85456F8C7599}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="87" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8750300" y="18745200"/>
+          <a:ext cx="965200" cy="469900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>167369</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="80" name="Straight Arrow Connector 79">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1FF61DF-CF63-0047-8826-07FF6DDD28D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="77" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6184900" y="19064969"/>
+          <a:ext cx="1104900" cy="73931"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="83" name="Rectangle 82">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA1555BF-A903-0C42-8857-461C35B9ECE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8496300" y="18884900"/>
+          <a:ext cx="863600" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>②-2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="84" name="Group 83">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{117E2C5F-32EC-FF43-AA7F-AB69816D2F72}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9715500" y="17399000"/>
+          <a:ext cx="2120900" cy="3632200"/>
+          <a:chOff x="9906000" y="16459200"/>
+          <a:chExt cx="5655022" cy="10058400"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="87" name="Picture 86">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC34B4E2-835C-D74B-7BE3-256E42651336}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9906000" y="16459200"/>
+            <a:ext cx="5655022" cy="10058400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="88" name="Picture 87">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E045A3C3-E44D-BE2A-786A-8E2557C47A31}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10223500" y="23050500"/>
+            <a:ext cx="5003800" cy="3429000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="89" name="Rectangle 88">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9D2218F-A869-1047-AA36-4C78286E8F55}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10121900" y="17030700"/>
+          <a:ext cx="1358900" cy="596900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="25400" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="6E747A">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>購入ページ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="92" name="Straight Arrow Connector 91">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68E07334-9F5A-234C-B9D3-73EF3830AADB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="75" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2070100" y="19037300"/>
+          <a:ext cx="2527300" cy="825500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="96" name="Straight Arrow Connector 95">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22E687C9-8983-0C49-A55B-29B472AC2F3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="75" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2057400" y="19037300"/>
+          <a:ext cx="2540000" cy="1765300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="105" name="Rounded Rectangle 104">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A044F972-7E48-5E49-BF44-D570889A0853}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3886200" y="22059900"/>
+          <a:ext cx="3022600" cy="4635500"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 4327"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="accent2"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Secure</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>WebView</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="106" name="Rectangle 105">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{999B2E19-477E-5141-BA45-B7A9D8A024AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4114800" y="22123400"/>
+          <a:ext cx="2590800" cy="4203700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Amazon側の画面</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>141427</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="104" name="Picture 103">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{871B7389-ABBF-CD4A-BDCC-030C0C49C116}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4394200" y="22491700"/>
+          <a:ext cx="1943100" cy="3456127"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>182338</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="107" name="Picture 106">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{293460A3-B768-3B06-4FCE-E15D48F998D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7150100" y="22555200"/>
+          <a:ext cx="1930400" cy="3433538"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>91169</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="108" name="Straight Arrow Connector 107">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{048532B1-5965-194B-840F-EB568096EF30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="107" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5410200" y="24271969"/>
+          <a:ext cx="1739900" cy="1166131"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5800,9 +8658,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5840,7 +8698,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5946,7 +8804,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6088,7 +8946,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6096,14 +8954,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96EB7A0-F1B0-DA4F-B651-30ECF70371F9}">
-  <dimension ref="A1"/>
+  <dimension ref="A108:A133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="108" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="109" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="110" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="111" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="112" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="113" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="114" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="115" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="116" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="117" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="118" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="119" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="120" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="121" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="122" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="123" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="124" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="125" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="126" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="127" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="128" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="129" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="130" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="131" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="132" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="133" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>